<commit_message>
found fairly good parameters
</commit_message>
<xml_diff>
--- a/ugeopgaver/2018-19/src/experimentWAninalsOutput.xlsx
+++ b/ugeopgaver/2018-19/src/experimentWAninalsOutput.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP/ugeopgaver/2018-19/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{078A2AD1-4D81-3640-9783-4DED46FE1804}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{759682A3-293D-424B-B4C8-3B03B0466F3D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{C0189421-3D8B-F643-96FD-9874918DA187}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{39EDBFD0-2388-054B-A4DA-58A9013216EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="test" localSheetId="0">Sheet1!$A$1:$C$100</definedName>
+    <definedName name="test" localSheetId="0">Sheet1!$A$1:$C$40</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +29,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{47C33025-601A-8445-9AF2-DD93A4B759F8}" name="test" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{BDD0094F-4197-8547-A32C-D777F13D1AF0}" name="test" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/sporring/repositories/PoP/ugeopgaver/2018-19/src/test.txt" decimal="," thousands="." comma="1">
       <textFields count="3">
         <textField/>
@@ -137,13 +137,26 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.6580927384076991E-2"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.88279768153980764"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Moose</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -156,311 +169,139 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Ticks</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$101</c:f>
+              <c:f>Sheet1!$B$1:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="101"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="33">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="34">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="35">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="36">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="38">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="39">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -468,13 +309,16 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F3BF-3346-A3C9-C4224EACE708}"/>
+              <c16:uniqueId val="{00000000-02D6-9E41-BB57-F63F13BBF279}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Wolves</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -487,107 +331,115 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Ticks</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$101</c:f>
+              <c:f>Sheet1!$C$1:$C$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="101"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>5</c:v>
@@ -596,202 +448,22 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -799,7 +471,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-F3BF-3346-A3C9-C4224EACE708}"/>
+              <c16:uniqueId val="{00000001-02D6-9E41-BB57-F63F13BBF279}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -812,16 +484,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1859214447"/>
-        <c:axId val="1859216127"/>
+        <c:axId val="1895962079"/>
+        <c:axId val="1896148975"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1859214447"/>
+        <c:axId val="1895962079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -858,7 +531,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1859216127"/>
+        <c:crossAx val="1896148975"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -866,7 +539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1859216127"/>
+        <c:axId val="1896148975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +590,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1859214447"/>
+        <c:crossAx val="1895962079"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -929,6 +602,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76977734033245859"/>
+          <c:y val="0.17208260425780114"/>
+          <c:w val="0.15800043744531933"/>
+          <c:h val="0.15625109361329836"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1533,23 +1247,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A73CB87-7795-D147-9578-F85461EB3A8C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{289730B7-B63E-1D42-8AFB-A4D8B481D6E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1285,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="test" connectionId="1" xr16:uid="{27C37571-084E-184E-893E-C3463CEFF606}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="test" connectionId="1" xr16:uid="{123B072D-50D3-B54B-8B25-2C8DF8F093A0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1870,18 +1584,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68153C9-C94F-9948-B5AF-C4BA6BFD5099}">
-  <dimension ref="A1:C100"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DF8B01-F1F9-AE4E-AC6B-FF82A13A11C4}">
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1889,10 +1601,10 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1900,10 +1612,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1911,10 +1623,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1922,10 +1634,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1933,10 +1645,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1944,10 +1656,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1955,7 +1667,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -1966,10 +1678,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1977,10 +1689,10 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1988,10 +1700,10 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1999,10 +1711,10 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2010,10 +1722,10 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2021,10 +1733,10 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2032,10 +1744,10 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2043,10 +1755,10 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2054,10 +1766,10 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2065,10 +1777,10 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2076,10 +1788,10 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2087,10 +1799,10 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2098,10 +1810,10 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2109,10 +1821,10 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2120,10 +1832,10 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2131,10 +1843,10 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2142,10 +1854,10 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2153,10 +1865,10 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C25">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2164,7 +1876,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>8</v>
@@ -2175,10 +1887,10 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2186,10 +1898,10 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2197,10 +1909,10 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2208,10 +1920,10 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2219,10 +1931,10 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2230,10 +1942,10 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2241,7 +1953,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -2252,7 +1964,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>5</v>
@@ -2263,10 +1975,10 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2274,10 +1986,10 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2285,10 +1997,10 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2296,10 +2008,10 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2307,10 +2019,10 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2318,670 +2030,10 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>41</v>
-      </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>42</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>43</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>44</v>
-      </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>45</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>46</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>47</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>48</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>49</v>
-      </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>50</v>
-      </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
-      <c r="C50">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>51</v>
-      </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="C51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>52</v>
-      </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
-      <c r="C52">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>53</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>54</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>55</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-      <c r="C55">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>56</v>
-      </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>57</v>
-      </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
-      <c r="C57">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>58</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="C58">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>59</v>
-      </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="C59">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>60</v>
-      </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
-      <c r="C60">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>61</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>62</v>
-      </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-      <c r="C62">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>63</v>
-      </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-      <c r="C63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>64</v>
-      </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
-      <c r="C64">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>65</v>
-      </c>
-      <c r="B65">
-        <v>0</v>
-      </c>
-      <c r="C65">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>66</v>
-      </c>
-      <c r="B66">
-        <v>0</v>
-      </c>
-      <c r="C66">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>67</v>
-      </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
-      <c r="C67">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>68</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>69</v>
-      </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
-      <c r="C69">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>70</v>
-      </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
-      <c r="C70">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>71</v>
-      </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-      <c r="C71">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>72</v>
-      </c>
-      <c r="B72">
-        <v>0</v>
-      </c>
-      <c r="C72">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>73</v>
-      </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="C73">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>74</v>
-      </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
-      <c r="C74">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>75</v>
-      </c>
-      <c r="B75">
-        <v>0</v>
-      </c>
-      <c r="C75">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>76</v>
-      </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="C76">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>77</v>
-      </c>
-      <c r="B77">
-        <v>0</v>
-      </c>
-      <c r="C77">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>78</v>
-      </c>
-      <c r="B78">
-        <v>0</v>
-      </c>
-      <c r="C78">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>79</v>
-      </c>
-      <c r="B79">
-        <v>0</v>
-      </c>
-      <c r="C79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>80</v>
-      </c>
-      <c r="B80">
-        <v>0</v>
-      </c>
-      <c r="C80">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>81</v>
-      </c>
-      <c r="B81">
-        <v>0</v>
-      </c>
-      <c r="C81">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>82</v>
-      </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
-      <c r="C82">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>83</v>
-      </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>84</v>
-      </c>
-      <c r="B84">
-        <v>0</v>
-      </c>
-      <c r="C84">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>85</v>
-      </c>
-      <c r="B85">
-        <v>0</v>
-      </c>
-      <c r="C85">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>86</v>
-      </c>
-      <c r="B86">
-        <v>0</v>
-      </c>
-      <c r="C86">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>87</v>
-      </c>
-      <c r="B87">
-        <v>0</v>
-      </c>
-      <c r="C87">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>88</v>
-      </c>
-      <c r="B88">
-        <v>0</v>
-      </c>
-      <c r="C88">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>89</v>
-      </c>
-      <c r="B89">
-        <v>0</v>
-      </c>
-      <c r="C89">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>90</v>
-      </c>
-      <c r="B90">
-        <v>0</v>
-      </c>
-      <c r="C90">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>91</v>
-      </c>
-      <c r="B91">
-        <v>0</v>
-      </c>
-      <c r="C91">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>92</v>
-      </c>
-      <c r="B92">
-        <v>0</v>
-      </c>
-      <c r="C92">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>93</v>
-      </c>
-      <c r="B93">
-        <v>0</v>
-      </c>
-      <c r="C93">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>94</v>
-      </c>
-      <c r="B94">
-        <v>0</v>
-      </c>
-      <c r="C94">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>95</v>
-      </c>
-      <c r="B95">
-        <v>0</v>
-      </c>
-      <c r="C95">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>96</v>
-      </c>
-      <c r="B96">
-        <v>0</v>
-      </c>
-      <c r="C96">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>97</v>
-      </c>
-      <c r="B97">
-        <v>0</v>
-      </c>
-      <c r="C97">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>98</v>
-      </c>
-      <c r="B98">
-        <v>0</v>
-      </c>
-      <c r="C98">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>99</v>
-      </c>
-      <c r="B99">
-        <v>0</v>
-      </c>
-      <c r="C99">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>100</v>
-      </c>
-      <c r="B100">
-        <v>0</v>
-      </c>
-      <c r="C100">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>